<commit_message>
Added support for AnsioU in mmCIF and fixed some issues with it
</commit_message>
<xml_diff>
--- a/pictures/support_overview.xlsx
+++ b/pictures/support_overview.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\douwe\Sources\pdbtbx\dump\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\douwe\Sources\pdbtbx\pictures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8EB702-B8E2-420F-ABA5-244556621E95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480E5FBB-3128-43FD-8AB9-AA21A407DF7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{98026335-BBEA-466D-9E49-FC174758B530}"/>
   </bookViews>
@@ -248,9 +248,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -281,14 +278,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,14 +853,14 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="5" width="5.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="13" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
@@ -869,155 +869,155 @@
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="11" t="s">
         <v>42</v>
       </c>
       <c r="G1" s="2"/>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="9"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L6" t="s">
@@ -1025,330 +1025,330 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="13" t="s">
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="13" t="s">
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="13" t="s">
+      <c r="D12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="13" t="s">
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="13" t="s">
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="13" t="s">
+      <c r="B16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="13" t="s">
+      <c r="B19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
@@ -1359,45 +1359,45 @@
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
@@ -1408,45 +1408,45 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
@@ -1457,45 +1457,45 @@
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="13" t="s">
+      <c r="B31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
@@ -1523,7 +1523,7 @@
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1 B2:E17 B22:G22 B25:G25 D1 F1:G17 B19:G19 B28:G28 B31:G31">
+  <conditionalFormatting sqref="B1 B22:G22 B25:G25 D1 F1:G17 B19:G19 B28:G28 B31:G31 B2:E17">
     <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
       <formula>"Support envisioned"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added support for DBREF1/2
</commit_message>
<xml_diff>
--- a/pictures/support_overview.xlsx
+++ b/pictures/support_overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\douwe\Sources\pdbtbx\pictures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480E5FBB-3128-43FD-8AB9-AA21A407DF7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E8ED4D-A443-4F81-9924-4DFF0C723DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{98026335-BBEA-466D-9E49-FC174758B530}"/>
   </bookViews>
@@ -853,7 +853,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,10 +1190,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>28</v>

</xml_diff>